<commit_message>
feat: new collum at book page, adjustments at all scripts
</commit_message>
<xml_diff>
--- a/listareduzida.xlsx
+++ b/listareduzida.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\book-fair\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2FBC15A-C676-4CA7-ACCA-61ED24AB44FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6A8F812-BA85-488C-8B3C-3B61825914BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="480" windowWidth="38640" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-38520" yWindow="585" windowWidth="38640" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="lista triagem 2024" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'lista triagem 2024'!$A$1:$G$251</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'lista triagem 2024'!$A$1:$H$251</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="758" uniqueCount="307">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="759" uniqueCount="308">
   <si>
     <t>Código FLE</t>
   </si>
@@ -950,6 +950,9 @@
   </si>
   <si>
     <t>Qual a sua dúvida para o tema: A Espiritualidade dos animais</t>
+  </si>
+  <si>
+    <t>Distribuidor</t>
   </si>
 </sst>
 </file>
@@ -1086,7 +1089,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="43" fontId="2" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1167,9 +1170,6 @@
     </xf>
     <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -1455,11 +1455,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G251"/>
+  <dimension ref="A1:H251"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A156" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C226" sqref="C226"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="K22" sqref="K22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1468,10 +1468,10 @@
     <col min="4" max="4" width="11.5703125" customWidth="1"/>
     <col min="5" max="5" width="48.7109375" customWidth="1"/>
     <col min="6" max="6" width="15.42578125" customWidth="1"/>
-    <col min="7" max="7" width="17.28515625" customWidth="1"/>
+    <col min="8" max="8" width="17.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1484,17 +1484,20 @@
       <c r="D1" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="31" t="s">
+      <c r="E1" s="8" t="s">
         <v>4</v>
       </c>
       <c r="F1" s="16" t="s">
         <v>10</v>
       </c>
       <c r="G1" s="16" t="s">
+        <v>307</v>
+      </c>
+      <c r="H1" s="16" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="3">
         <v>4</v>
       </c>
@@ -1513,11 +1516,11 @@
       <c r="F2" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="G2" s="17" t="s">
+      <c r="H2" s="17" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="3">
         <v>6</v>
       </c>
@@ -1536,11 +1539,11 @@
       <c r="F3" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="G3" s="17" t="s">
+      <c r="H3" s="17" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="3">
         <v>7</v>
       </c>
@@ -1559,11 +1562,11 @@
       <c r="F4" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="G4" s="17" t="s">
+      <c r="H4" s="17" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="3">
         <v>13</v>
       </c>
@@ -1582,11 +1585,11 @@
       <c r="F5" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="G5" s="17" t="s">
+      <c r="H5" s="17" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="3">
         <v>30</v>
       </c>
@@ -1605,11 +1608,11 @@
       <c r="F6" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="G6" s="17" t="s">
+      <c r="H6" s="17" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="3">
         <v>45</v>
       </c>
@@ -1628,11 +1631,11 @@
       <c r="F7" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="G7" s="17" t="s">
+      <c r="H7" s="17" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="3">
         <v>50</v>
       </c>
@@ -1651,11 +1654,11 @@
       <c r="F8" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="G8" s="17" t="s">
+      <c r="H8" s="17" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="3">
         <v>53</v>
       </c>
@@ -1674,11 +1677,11 @@
       <c r="F9" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="G9" s="17" t="s">
+      <c r="H9" s="17" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="3">
         <v>64</v>
       </c>
@@ -1697,11 +1700,11 @@
       <c r="F10" s="13" t="s">
         <v>39</v>
       </c>
-      <c r="G10" s="17" t="s">
+      <c r="H10" s="17" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="3">
         <v>67</v>
       </c>
@@ -1720,11 +1723,11 @@
       <c r="F11" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="G11" s="17" t="s">
+      <c r="H11" s="17" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="3">
         <v>69</v>
       </c>
@@ -1743,11 +1746,11 @@
       <c r="F12" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="G12" s="17" t="s">
+      <c r="H12" s="17" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="3">
         <v>72</v>
       </c>
@@ -1766,11 +1769,11 @@
       <c r="F13" s="13" t="s">
         <v>39</v>
       </c>
-      <c r="G13" s="17" t="s">
+      <c r="H13" s="17" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="3">
         <v>75</v>
       </c>
@@ -1789,11 +1792,11 @@
       <c r="F14" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="G14" s="17" t="s">
+      <c r="H14" s="17" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="3">
         <v>77</v>
       </c>
@@ -1812,11 +1815,11 @@
       <c r="F15" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="G15" s="17" t="s">
+      <c r="H15" s="17" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="3">
         <v>81</v>
       </c>
@@ -1835,11 +1838,11 @@
       <c r="F16" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="G16" s="17" t="s">
+      <c r="H16" s="17" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="3">
         <v>84</v>
       </c>
@@ -1858,11 +1861,11 @@
       <c r="F17" s="13" t="s">
         <v>59</v>
       </c>
-      <c r="G17" s="17" t="s">
+      <c r="H17" s="17" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="3">
         <v>89</v>
       </c>
@@ -1881,11 +1884,11 @@
       <c r="F18" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="G18" s="17" t="s">
+      <c r="H18" s="17" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="3">
         <v>93</v>
       </c>
@@ -1904,11 +1907,11 @@
       <c r="F19" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="G19" s="17" t="s">
+      <c r="H19" s="17" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="3">
         <v>94</v>
       </c>
@@ -1927,11 +1930,11 @@
       <c r="F20" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="G20" s="17" t="s">
+      <c r="H20" s="17" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="3">
         <v>106</v>
       </c>
@@ -1950,11 +1953,11 @@
       <c r="F21" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="G21" s="17" t="s">
+      <c r="H21" s="17" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="3">
         <v>114</v>
       </c>
@@ -1973,11 +1976,11 @@
       <c r="F22" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="G22" s="17" t="s">
+      <c r="H22" s="17" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="3">
         <v>119</v>
       </c>
@@ -1996,11 +1999,11 @@
       <c r="F23" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="G23" s="17" t="s">
+      <c r="H23" s="17" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="3">
         <v>120</v>
       </c>
@@ -2019,11 +2022,11 @@
       <c r="F24" s="13" t="s">
         <v>65</v>
       </c>
-      <c r="G24" s="17" t="s">
+      <c r="H24" s="17" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="3">
         <v>121</v>
       </c>
@@ -2042,11 +2045,11 @@
       <c r="F25" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="G25" s="17" t="s">
+      <c r="H25" s="17" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="3">
         <v>125</v>
       </c>
@@ -2065,11 +2068,11 @@
       <c r="F26" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="G26" s="17" t="s">
+      <c r="H26" s="17" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" s="3">
         <v>128</v>
       </c>
@@ -2088,11 +2091,11 @@
       <c r="F27" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="G27" s="17" t="s">
+      <c r="H27" s="17" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" s="3">
         <v>133</v>
       </c>
@@ -2111,11 +2114,11 @@
       <c r="F28" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="G28" s="17" t="s">
+      <c r="H28" s="17" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" s="3">
         <v>137</v>
       </c>
@@ -2134,11 +2137,11 @@
       <c r="F29" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="G29" s="17" t="s">
+      <c r="H29" s="17" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" s="3">
         <v>138</v>
       </c>
@@ -2157,11 +2160,11 @@
       <c r="F30" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="G30" s="17" t="s">
+      <c r="H30" s="17" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" s="3">
         <v>141</v>
       </c>
@@ -2180,11 +2183,11 @@
       <c r="F31" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="G31" s="17" t="s">
+      <c r="H31" s="17" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" s="3">
         <v>151</v>
       </c>
@@ -2203,11 +2206,11 @@
       <c r="F32" s="13" t="s">
         <v>62</v>
       </c>
-      <c r="G32" s="17" t="s">
+      <c r="H32" s="17" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" s="3">
         <v>152</v>
       </c>
@@ -2226,11 +2229,11 @@
       <c r="F33" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="G33" s="17" t="s">
+      <c r="H33" s="17" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" s="3">
         <v>156</v>
       </c>
@@ -2249,11 +2252,11 @@
       <c r="F34" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="G34" s="17" t="s">
+      <c r="H34" s="17" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" s="3">
         <v>158</v>
       </c>
@@ -2272,11 +2275,11 @@
       <c r="F35" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="G35" s="17" t="s">
+      <c r="H35" s="17" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" s="3">
         <v>160</v>
       </c>
@@ -2295,11 +2298,11 @@
       <c r="F36" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="G36" s="17" t="s">
+      <c r="H36" s="17" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" s="3">
         <v>163</v>
       </c>
@@ -2318,11 +2321,11 @@
       <c r="F37" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="G37" s="17" t="s">
+      <c r="H37" s="17" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" s="3">
         <v>164</v>
       </c>
@@ -2341,11 +2344,11 @@
       <c r="F38" s="13" t="s">
         <v>76</v>
       </c>
-      <c r="G38" s="17" t="s">
+      <c r="H38" s="17" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" s="3">
         <v>167</v>
       </c>
@@ -2364,11 +2367,11 @@
       <c r="F39" s="13" t="s">
         <v>65</v>
       </c>
-      <c r="G39" s="17" t="s">
+      <c r="H39" s="17" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" s="3">
         <v>177</v>
       </c>
@@ -2387,11 +2390,11 @@
       <c r="F40" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="G40" s="17" t="s">
+      <c r="H40" s="17" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41" s="3">
         <v>178</v>
       </c>
@@ -2410,11 +2413,11 @@
       <c r="F41" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="G41" s="17" t="s">
+      <c r="H41" s="17" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42" s="3">
         <v>182</v>
       </c>
@@ -2433,11 +2436,11 @@
       <c r="F42" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="G42" s="17" t="s">
+      <c r="H42" s="17" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43" s="3">
         <v>195</v>
       </c>
@@ -2456,11 +2459,11 @@
       <c r="F43" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="G43" s="17" t="s">
+      <c r="H43" s="17" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A44" s="3">
         <v>196</v>
       </c>
@@ -2479,11 +2482,11 @@
       <c r="F44" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="G44" s="17" t="s">
+      <c r="H44" s="17" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A45" s="3">
         <v>197</v>
       </c>
@@ -2502,11 +2505,11 @@
       <c r="F45" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="G45" s="17" t="s">
+      <c r="H45" s="17" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A46" s="3">
         <v>203</v>
       </c>
@@ -2525,11 +2528,11 @@
       <c r="F46" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="G46" s="17" t="s">
+      <c r="H46" s="17" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A47" s="3">
         <v>221</v>
       </c>
@@ -2548,11 +2551,11 @@
       <c r="F47" s="17" t="s">
         <v>102</v>
       </c>
-      <c r="G47" s="17" t="s">
+      <c r="H47" s="17" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A48" s="3">
         <v>223</v>
       </c>
@@ -2571,11 +2574,11 @@
       <c r="F48" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="G48" s="17" t="s">
+      <c r="H48" s="17" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A49" s="3">
         <v>232</v>
       </c>
@@ -2594,11 +2597,11 @@
       <c r="F49" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="G49" s="17" t="s">
+      <c r="H49" s="17" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A50" s="3">
         <v>233</v>
       </c>
@@ -2617,11 +2620,11 @@
       <c r="F50" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="G50" s="17" t="s">
+      <c r="H50" s="17" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A51" s="3">
         <v>234</v>
       </c>
@@ -2640,11 +2643,11 @@
       <c r="F51" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="G51" s="17" t="s">
+      <c r="H51" s="17" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A52" s="3">
         <v>235</v>
       </c>
@@ -2663,11 +2666,11 @@
       <c r="F52" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="G52" s="17" t="s">
+      <c r="H52" s="17" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A53" s="3">
         <v>239</v>
       </c>
@@ -2686,11 +2689,11 @@
       <c r="F53" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="G53" s="17" t="s">
+      <c r="H53" s="17" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A54" s="3">
         <v>242</v>
       </c>
@@ -2709,11 +2712,11 @@
       <c r="F54" s="13" t="s">
         <v>105</v>
       </c>
-      <c r="G54" s="17" t="s">
+      <c r="H54" s="17" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A55" s="3">
         <v>243</v>
       </c>
@@ -2730,11 +2733,11 @@
       <c r="F55" s="13" t="s">
         <v>65</v>
       </c>
-      <c r="G55" s="17" t="s">
+      <c r="H55" s="17" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A56" s="3">
         <v>245</v>
       </c>
@@ -2753,11 +2756,11 @@
       <c r="F56" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="G56" s="17" t="s">
+      <c r="H56" s="17" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A57" s="3">
         <v>248</v>
       </c>
@@ -2776,11 +2779,11 @@
       <c r="F57" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="G57" s="17" t="s">
+      <c r="H57" s="17" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A58" s="3">
         <v>253</v>
       </c>
@@ -2799,11 +2802,11 @@
       <c r="F58" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="G58" s="17" t="s">
+      <c r="H58" s="17" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A59" s="3">
         <v>256</v>
       </c>
@@ -2822,11 +2825,11 @@
       <c r="F59" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="G59" s="17" t="s">
+      <c r="H59" s="17" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A60" s="3">
         <v>266</v>
       </c>
@@ -2845,11 +2848,11 @@
       <c r="F60" s="13" t="s">
         <v>63</v>
       </c>
-      <c r="G60" s="17" t="s">
+      <c r="H60" s="17" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A61" s="3">
         <v>284</v>
       </c>
@@ -2868,11 +2871,11 @@
       <c r="F61" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="G61" s="17" t="s">
+      <c r="H61" s="17" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A62" s="3">
         <v>287</v>
       </c>
@@ -2891,11 +2894,11 @@
       <c r="F62" s="13" t="s">
         <v>107</v>
       </c>
-      <c r="G62" s="17" t="s">
+      <c r="H62" s="17" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A63" s="3">
         <v>292</v>
       </c>
@@ -2914,11 +2917,11 @@
       <c r="F63" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="G63" s="17" t="s">
+      <c r="H63" s="17" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A64" s="3">
         <v>297</v>
       </c>
@@ -2937,11 +2940,11 @@
       <c r="F64" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="G64" s="17" t="s">
+      <c r="H64" s="17" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A65" s="3">
         <v>298</v>
       </c>
@@ -2960,11 +2963,11 @@
       <c r="F65" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="G65" s="17" t="s">
+      <c r="H65" s="17" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A66" s="3">
         <v>305</v>
       </c>
@@ -2983,11 +2986,11 @@
       <c r="F66" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="G66" s="17" t="s">
+      <c r="H66" s="17" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="67" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A67" s="3">
         <v>314</v>
       </c>
@@ -3006,11 +3009,11 @@
       <c r="F67" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="G67" s="17" t="s">
+      <c r="H67" s="17" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="68" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A68" s="3">
         <v>328</v>
       </c>
@@ -3029,11 +3032,11 @@
       <c r="F68" s="13" t="s">
         <v>65</v>
       </c>
-      <c r="G68" s="17" t="s">
+      <c r="H68" s="17" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="69" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A69" s="3">
         <v>334</v>
       </c>
@@ -3052,11 +3055,11 @@
       <c r="F69" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="G69" s="17" t="s">
+      <c r="H69" s="17" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="70" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A70" s="3">
         <v>335</v>
       </c>
@@ -3075,11 +3078,11 @@
       <c r="F70" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="G70" s="17" t="s">
+      <c r="H70" s="17" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="71" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A71" s="3">
         <v>339</v>
       </c>
@@ -3098,11 +3101,11 @@
       <c r="F71" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="G71" s="17" t="s">
+      <c r="H71" s="17" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="72" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A72" s="3">
         <v>345</v>
       </c>
@@ -3121,11 +3124,11 @@
       <c r="F72" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="G72" s="17" t="s">
+      <c r="H72" s="17" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="73" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A73" s="3">
         <v>351</v>
       </c>
@@ -3144,11 +3147,11 @@
       <c r="F73" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="G73" s="17" t="s">
+      <c r="H73" s="17" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="74" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A74" s="3">
         <v>360</v>
       </c>
@@ -3167,11 +3170,11 @@
       <c r="F74" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="G74" s="17" t="s">
+      <c r="H74" s="17" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="75" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A75" s="3">
         <v>364</v>
       </c>
@@ -3190,11 +3193,11 @@
       <c r="F75" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="G75" s="17" t="s">
+      <c r="H75" s="17" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="76" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A76" s="3">
         <v>365</v>
       </c>
@@ -3213,11 +3216,11 @@
       <c r="F76" s="22" t="s">
         <v>12</v>
       </c>
-      <c r="G76" s="17" t="s">
+      <c r="H76" s="17" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="77" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A77" s="3">
         <v>369</v>
       </c>
@@ -3236,11 +3239,11 @@
       <c r="F77" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="G77" s="17" t="s">
+      <c r="H77" s="17" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="78" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A78" s="3">
         <v>371</v>
       </c>
@@ -3259,11 +3262,11 @@
       <c r="F78" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="G78" s="17" t="s">
+      <c r="H78" s="17" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="79" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A79" s="3">
         <v>389</v>
       </c>
@@ -3282,11 +3285,11 @@
       <c r="F79" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="G79" s="17" t="s">
+      <c r="H79" s="17" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="80" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A80" s="3">
         <v>391</v>
       </c>
@@ -3305,11 +3308,11 @@
       <c r="F80" s="13" t="s">
         <v>59</v>
       </c>
-      <c r="G80" s="17" t="s">
+      <c r="H80" s="17" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="81" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A81" s="3">
         <v>399</v>
       </c>
@@ -3328,11 +3331,11 @@
       <c r="F81" s="13" t="s">
         <v>65</v>
       </c>
-      <c r="G81" s="17" t="s">
+      <c r="H81" s="17" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="82" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A82" s="3">
         <v>403</v>
       </c>
@@ -3351,11 +3354,11 @@
       <c r="F82" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="G82" s="13" t="s">
+      <c r="H82" s="13" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="83" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A83" s="3">
         <v>407</v>
       </c>
@@ -3374,11 +3377,11 @@
       <c r="F83" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="G83" s="17" t="s">
+      <c r="H83" s="17" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="84" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A84" s="3">
         <v>410</v>
       </c>
@@ -3397,11 +3400,11 @@
       <c r="F84" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="G84" s="17" t="s">
+      <c r="H84" s="17" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="85" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A85" s="3">
         <v>417</v>
       </c>
@@ -3420,11 +3423,11 @@
       <c r="F85" s="13" t="s">
         <v>133</v>
       </c>
-      <c r="G85" s="17" t="s">
+      <c r="H85" s="17" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="86" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A86" s="3">
         <v>421</v>
       </c>
@@ -3443,11 +3446,11 @@
       <c r="F86" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="G86" s="17" t="s">
+      <c r="H86" s="17" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="87" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A87" s="3">
         <v>449</v>
       </c>
@@ -3466,11 +3469,11 @@
       <c r="F87" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="G87" s="17" t="s">
+      <c r="H87" s="17" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="88" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A88" s="3">
         <v>452</v>
       </c>
@@ -3489,11 +3492,11 @@
       <c r="F88" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="G88" s="17" t="s">
+      <c r="H88" s="17" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="89" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A89" s="3">
         <v>453</v>
       </c>
@@ -3512,11 +3515,11 @@
       <c r="F89" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="G89" s="17" t="s">
+      <c r="H89" s="17" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="90" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A90" s="23">
         <v>456</v>
       </c>
@@ -3535,11 +3538,11 @@
       <c r="F90" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="G90" s="17" t="s">
+      <c r="H90" s="17" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="91" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A91" s="3">
         <v>460</v>
       </c>
@@ -3558,11 +3561,11 @@
       <c r="F91" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="G91" s="17" t="s">
+      <c r="H91" s="17" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="92" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A92" s="3">
         <v>466</v>
       </c>
@@ -3581,11 +3584,11 @@
       <c r="F92" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="G92" s="17" t="s">
+      <c r="H92" s="17" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="93" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A93" s="3">
         <v>467</v>
       </c>
@@ -3604,11 +3607,11 @@
       <c r="F93" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="G93" s="17" t="s">
+      <c r="H93" s="17" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="94" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A94" s="3">
         <v>475</v>
       </c>
@@ -3627,11 +3630,11 @@
       <c r="F94" s="13" t="s">
         <v>40</v>
       </c>
-      <c r="G94" s="17" t="s">
+      <c r="H94" s="17" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="95" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A95" s="3">
         <v>476</v>
       </c>
@@ -3650,11 +3653,11 @@
       <c r="F95" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="G95" s="17" t="s">
+      <c r="H95" s="17" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="96" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A96" s="3">
         <v>477</v>
       </c>
@@ -3673,11 +3676,11 @@
       <c r="F96" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="G96" s="17" t="s">
+      <c r="H96" s="17" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="97" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A97" s="3">
         <v>478</v>
       </c>
@@ -3696,11 +3699,11 @@
       <c r="F97" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="G97" s="17" t="s">
+      <c r="H97" s="17" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="98" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A98" s="3">
         <v>479</v>
       </c>
@@ -3719,11 +3722,11 @@
       <c r="F98" s="13" t="s">
         <v>38</v>
       </c>
-      <c r="G98" s="17" t="s">
+      <c r="H98" s="17" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="99" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A99" s="3">
         <v>485</v>
       </c>
@@ -3742,11 +3745,11 @@
       <c r="F99" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="G99" s="13" t="s">
+      <c r="H99" s="13" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="100" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A100" s="3">
         <v>486</v>
       </c>
@@ -3765,11 +3768,11 @@
       <c r="F100" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="G100" s="17" t="s">
+      <c r="H100" s="17" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="101" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A101" s="3">
         <v>489</v>
       </c>
@@ -3788,11 +3791,11 @@
       <c r="F101" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="G101" s="17" t="s">
+      <c r="H101" s="17" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="102" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A102" s="3">
         <v>490</v>
       </c>
@@ -3805,17 +3808,17 @@
       <c r="D102" s="20">
         <v>50</v>
       </c>
-      <c r="E102" s="32" t="s">
+      <c r="E102" s="31" t="s">
         <v>150</v>
       </c>
       <c r="F102" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="G102" s="17" t="s">
+      <c r="H102" s="17" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="103" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A103" s="3">
         <v>492</v>
       </c>
@@ -3834,11 +3837,11 @@
       <c r="F103" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="G103" s="17" t="s">
+      <c r="H103" s="17" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="104" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A104" s="3">
         <v>505</v>
       </c>
@@ -3857,11 +3860,11 @@
       <c r="F104" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="G104" s="17" t="s">
+      <c r="H104" s="17" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="105" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A105" s="3">
         <v>506</v>
       </c>
@@ -3880,11 +3883,11 @@
       <c r="F105" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="G105" s="17" t="s">
+      <c r="H105" s="17" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="106" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A106" s="3">
         <v>512</v>
       </c>
@@ -3903,11 +3906,11 @@
       <c r="F106" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="G106" s="17" t="s">
+      <c r="H106" s="17" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="107" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A107" s="3">
         <v>520</v>
       </c>
@@ -3926,11 +3929,11 @@
       <c r="F107" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="G107" s="17" t="s">
+      <c r="H107" s="17" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="108" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A108" s="3">
         <v>521</v>
       </c>
@@ -3949,11 +3952,11 @@
       <c r="F108" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="G108" s="17" t="s">
+      <c r="H108" s="17" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="109" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A109" s="3">
         <v>524</v>
       </c>
@@ -3972,11 +3975,11 @@
       <c r="F109" s="13" t="s">
         <v>38</v>
       </c>
-      <c r="G109" s="17" t="s">
+      <c r="H109" s="17" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="110" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A110" s="3">
         <v>528</v>
       </c>
@@ -3995,11 +3998,11 @@
       <c r="F110" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="G110" s="17" t="s">
+      <c r="H110" s="17" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="111" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A111" s="3">
         <v>541</v>
       </c>
@@ -4018,11 +4021,11 @@
       <c r="F111" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="G111" s="17" t="s">
+      <c r="H111" s="17" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="112" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A112" s="3">
         <v>543</v>
       </c>
@@ -4035,17 +4038,17 @@
       <c r="D112" s="20">
         <v>42</v>
       </c>
-      <c r="E112" s="32" t="s">
+      <c r="E112" s="31" t="s">
         <v>163</v>
       </c>
       <c r="F112" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="G112" s="17" t="s">
+      <c r="H112" s="17" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="113" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A113" s="3">
         <v>547</v>
       </c>
@@ -4064,11 +4067,11 @@
       <c r="F113" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="G113" s="17" t="s">
+      <c r="H113" s="17" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="114" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A114" s="3">
         <v>556</v>
       </c>
@@ -4087,11 +4090,11 @@
       <c r="F114" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="G114" s="17" t="s">
+      <c r="H114" s="17" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="115" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A115" s="3">
         <v>558</v>
       </c>
@@ -4110,11 +4113,11 @@
       <c r="F115" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="G115" s="17" t="s">
+      <c r="H115" s="17" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="116" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A116" s="3">
         <v>560</v>
       </c>
@@ -4133,11 +4136,11 @@
       <c r="F116" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="G116" s="17" t="s">
+      <c r="H116" s="17" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="117" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A117" s="3">
         <v>562</v>
       </c>
@@ -4156,11 +4159,11 @@
       <c r="F117" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="G117" s="17" t="s">
+      <c r="H117" s="17" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="118" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A118" s="18">
         <v>567</v>
       </c>
@@ -4179,11 +4182,11 @@
       <c r="F118" s="13" t="s">
         <v>171</v>
       </c>
-      <c r="G118" s="17" t="s">
+      <c r="H118" s="17" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="119" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A119" s="3">
         <v>570</v>
       </c>
@@ -4202,11 +4205,11 @@
       <c r="F119" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="G119" s="17" t="s">
+      <c r="H119" s="17" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="120" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A120" s="3">
         <v>572</v>
       </c>
@@ -4225,11 +4228,11 @@
       <c r="F120" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="G120" s="17" t="s">
+      <c r="H120" s="17" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="121" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A121" s="3">
         <v>580</v>
       </c>
@@ -4248,11 +4251,11 @@
       <c r="F121" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="G121" s="17" t="s">
+      <c r="H121" s="17" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="122" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A122" s="3">
         <v>587</v>
       </c>
@@ -4271,11 +4274,11 @@
       <c r="F122" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="G122" s="17" t="s">
+      <c r="H122" s="17" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="123" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A123" s="3">
         <v>588</v>
       </c>
@@ -4294,11 +4297,11 @@
       <c r="F123" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="G123" s="17" t="s">
+      <c r="H123" s="17" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="124" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A124" s="3">
         <v>589</v>
       </c>
@@ -4317,11 +4320,11 @@
       <c r="F124" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="G124" s="17" t="s">
+      <c r="H124" s="17" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="125" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A125" s="3">
         <v>592</v>
       </c>
@@ -4340,11 +4343,11 @@
       <c r="F125" s="13" t="s">
         <v>119</v>
       </c>
-      <c r="G125" s="17" t="s">
+      <c r="H125" s="17" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="126" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A126" s="3">
         <v>603</v>
       </c>
@@ -4363,11 +4366,11 @@
       <c r="F126" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="G126" s="17" t="s">
+      <c r="H126" s="17" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="127" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A127" s="3">
         <v>609</v>
       </c>
@@ -4386,11 +4389,11 @@
       <c r="F127" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="G127" s="17" t="s">
+      <c r="H127" s="17" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="128" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A128" s="3">
         <v>615</v>
       </c>
@@ -4409,11 +4412,11 @@
       <c r="F128" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="G128" s="17" t="s">
+      <c r="H128" s="17" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="129" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A129" s="3">
         <v>635</v>
       </c>
@@ -4432,11 +4435,11 @@
       <c r="F129" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="G129" s="17" t="s">
+      <c r="H129" s="17" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="130" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A130" s="3">
         <v>645</v>
       </c>
@@ -4455,11 +4458,11 @@
       <c r="F130" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="G130" s="17" t="s">
+      <c r="H130" s="17" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="131" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A131" s="3">
         <v>648</v>
       </c>
@@ -4478,11 +4481,11 @@
       <c r="F131" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="G131" s="17" t="s">
+      <c r="H131" s="17" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="132" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A132" s="3">
         <v>656</v>
       </c>
@@ -4501,11 +4504,11 @@
       <c r="F132" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="G132" s="17" t="s">
+      <c r="H132" s="17" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="133" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A133" s="3">
         <v>657</v>
       </c>
@@ -4524,11 +4527,11 @@
       <c r="F133" s="12" t="s">
         <v>59</v>
       </c>
-      <c r="G133" s="17" t="s">
+      <c r="H133" s="17" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="134" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A134" s="3">
         <v>662</v>
       </c>
@@ -4547,11 +4550,11 @@
       <c r="F134" s="19" t="s">
         <v>59</v>
       </c>
-      <c r="G134" s="19" t="s">
+      <c r="H134" s="19" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="135" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A135" s="3">
         <v>665</v>
       </c>
@@ -4570,11 +4573,11 @@
       <c r="F135" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="G135" s="19" t="s">
+      <c r="H135" s="19" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="136" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A136" s="3">
         <v>684</v>
       </c>
@@ -4593,11 +4596,11 @@
       <c r="F136" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="G136" s="17" t="s">
+      <c r="H136" s="17" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="137" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A137" s="3">
         <v>692</v>
       </c>
@@ -4616,11 +4619,11 @@
       <c r="F137" s="13" t="s">
         <v>38</v>
       </c>
-      <c r="G137" s="17" t="s">
+      <c r="H137" s="17" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="138" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A138" s="3">
         <v>695</v>
       </c>
@@ -4639,11 +4642,11 @@
       <c r="F138" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="G138" s="17" t="s">
+      <c r="H138" s="17" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="139" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A139" s="3">
         <v>702</v>
       </c>
@@ -4662,11 +4665,11 @@
       <c r="F139" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="G139" s="17" t="s">
+      <c r="H139" s="17" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="140" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A140" s="3">
         <v>726</v>
       </c>
@@ -4685,11 +4688,11 @@
       <c r="F140" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="G140" s="17" t="s">
+      <c r="H140" s="17" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="141" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A141" s="3">
         <v>732</v>
       </c>
@@ -4708,11 +4711,11 @@
       <c r="F141" s="13" t="s">
         <v>59</v>
       </c>
-      <c r="G141" s="17" t="s">
+      <c r="H141" s="17" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="142" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A142" s="3">
         <v>741</v>
       </c>
@@ -4731,11 +4734,11 @@
       <c r="F142" s="13" t="s">
         <v>159</v>
       </c>
-      <c r="G142" s="17" t="s">
+      <c r="H142" s="17" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="143" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A143" s="3">
         <v>755</v>
       </c>
@@ -4754,11 +4757,11 @@
       <c r="F143" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="G143" s="17" t="s">
+      <c r="H143" s="17" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="144" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A144" s="3">
         <v>760</v>
       </c>
@@ -4777,11 +4780,11 @@
       <c r="F144" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="G144" s="17" t="s">
+      <c r="H144" s="17" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="145" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A145" s="3">
         <v>780</v>
       </c>
@@ -4800,11 +4803,11 @@
       <c r="F145" s="19" t="s">
         <v>59</v>
       </c>
-      <c r="G145" s="19" t="s">
+      <c r="H145" s="19" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="146" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A146" s="3">
         <v>804</v>
       </c>
@@ -4823,11 +4826,11 @@
       <c r="F146" s="19" t="s">
         <v>38</v>
       </c>
-      <c r="G146" s="17" t="s">
+      <c r="H146" s="17" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="147" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A147" s="3">
         <v>809</v>
       </c>
@@ -4846,11 +4849,11 @@
       <c r="F147" s="13" t="s">
         <v>108</v>
       </c>
-      <c r="G147" s="17" t="s">
+      <c r="H147" s="17" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="148" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A148" s="3">
         <v>810</v>
       </c>
@@ -4869,11 +4872,11 @@
       <c r="F148" s="13" t="s">
         <v>38</v>
       </c>
-      <c r="G148" s="17" t="s">
+      <c r="H148" s="17" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="149" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A149" s="3">
         <v>822</v>
       </c>
@@ -4892,11 +4895,11 @@
       <c r="F149" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="G149" s="17" t="s">
+      <c r="H149" s="17" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="150" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A150" s="3">
         <v>824</v>
       </c>
@@ -4915,11 +4918,11 @@
       <c r="F150" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="G150" s="17" t="s">
+      <c r="H150" s="17" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="151" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A151" s="3">
         <v>825</v>
       </c>
@@ -4938,11 +4941,11 @@
       <c r="F151" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="G151" s="17" t="s">
+      <c r="H151" s="17" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="152" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A152" s="3">
         <v>826</v>
       </c>
@@ -4961,11 +4964,11 @@
       <c r="F152" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="G152" s="17" t="s">
+      <c r="H152" s="17" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="153" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A153" s="3">
         <v>832</v>
       </c>
@@ -4984,11 +4987,11 @@
       <c r="F153" s="13" t="s">
         <v>105</v>
       </c>
-      <c r="G153" s="17" t="s">
+      <c r="H153" s="17" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="154" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A154" s="3">
         <v>841</v>
       </c>
@@ -5007,11 +5010,11 @@
       <c r="F154" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="G154" s="17" t="s">
+      <c r="H154" s="17" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="155" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A155" s="3">
         <v>842</v>
       </c>
@@ -5030,11 +5033,11 @@
       <c r="F155" s="13" t="s">
         <v>159</v>
       </c>
-      <c r="G155" s="17" t="s">
+      <c r="H155" s="17" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="156" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A156" s="3">
         <v>845</v>
       </c>
@@ -5053,11 +5056,11 @@
       <c r="F156" s="13" t="s">
         <v>59</v>
       </c>
-      <c r="G156" s="17" t="s">
+      <c r="H156" s="17" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="157" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A157" s="3">
         <v>860</v>
       </c>
@@ -5076,11 +5079,11 @@
       <c r="F157" s="13" t="s">
         <v>59</v>
       </c>
-      <c r="G157" s="17" t="s">
+      <c r="H157" s="17" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="158" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A158" s="3">
         <v>884</v>
       </c>
@@ -5099,11 +5102,11 @@
       <c r="F158" s="13" t="s">
         <v>38</v>
       </c>
-      <c r="G158" s="17" t="s">
+      <c r="H158" s="17" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="159" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A159" s="3">
         <v>886</v>
       </c>
@@ -5122,11 +5125,11 @@
       <c r="F159" s="19" t="s">
         <v>65</v>
       </c>
-      <c r="G159" s="17" t="s">
+      <c r="H159" s="17" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="160" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A160" s="3">
         <v>888</v>
       </c>
@@ -5145,11 +5148,11 @@
       <c r="F160" s="13" t="s">
         <v>159</v>
       </c>
-      <c r="G160" s="17" t="s">
+      <c r="H160" s="17" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="161" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A161" s="3">
         <v>912</v>
       </c>
@@ -5168,11 +5171,11 @@
       <c r="F161" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="G161" s="17" t="s">
+      <c r="H161" s="17" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="162" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A162" s="3">
         <v>921</v>
       </c>
@@ -5191,11 +5194,11 @@
       <c r="F162" s="13" t="s">
         <v>108</v>
       </c>
-      <c r="G162" s="17" t="s">
+      <c r="H162" s="17" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="163" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A163" s="3">
         <v>922</v>
       </c>
@@ -5214,11 +5217,11 @@
       <c r="F163" s="13" t="s">
         <v>65</v>
       </c>
-      <c r="G163" s="17" t="s">
+      <c r="H163" s="17" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="164" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A164" s="3">
         <v>927</v>
       </c>
@@ -5237,11 +5240,11 @@
       <c r="F164" s="13" t="s">
         <v>59</v>
       </c>
-      <c r="G164" s="17" t="s">
+      <c r="H164" s="17" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="165" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A165" s="3">
         <v>975</v>
       </c>
@@ -5260,11 +5263,11 @@
       <c r="F165" s="13" t="s">
         <v>38</v>
       </c>
-      <c r="G165" s="17" t="s">
+      <c r="H165" s="17" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="166" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A166" s="3">
         <v>988</v>
       </c>
@@ -5283,11 +5286,11 @@
       <c r="F166" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="G166" s="17" t="s">
+      <c r="H166" s="17" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="167" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A167" s="3">
         <v>990</v>
       </c>
@@ -5306,11 +5309,11 @@
       <c r="F167" s="13" t="s">
         <v>59</v>
       </c>
-      <c r="G167" s="17" t="s">
+      <c r="H167" s="17" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="168" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A168" s="3">
         <v>1018</v>
       </c>
@@ -5329,11 +5332,11 @@
       <c r="F168" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="G168" s="17" t="s">
+      <c r="H168" s="17" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="169" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A169" s="3">
         <v>1037</v>
       </c>
@@ -5352,11 +5355,11 @@
       <c r="F169" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="G169" s="17" t="s">
+      <c r="H169" s="17" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="170" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A170" s="3">
         <v>1041</v>
       </c>
@@ -5375,11 +5378,11 @@
       <c r="F170" s="13" t="s">
         <v>222</v>
       </c>
-      <c r="G170" s="17" t="s">
+      <c r="H170" s="17" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="171" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A171" s="3">
         <v>1088</v>
       </c>
@@ -5398,11 +5401,11 @@
       <c r="F171" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="G171" s="17" t="s">
+      <c r="H171" s="17" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="172" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A172" s="3">
         <v>1091</v>
       </c>
@@ -5421,11 +5424,11 @@
       <c r="F172" s="13" t="s">
         <v>105</v>
       </c>
-      <c r="G172" s="17" t="s">
+      <c r="H172" s="17" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="173" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A173" s="3">
         <v>1110</v>
       </c>
@@ -5444,11 +5447,11 @@
       <c r="F173" s="13" t="s">
         <v>171</v>
       </c>
-      <c r="G173" s="13" t="s">
+      <c r="H173" s="13" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="174" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A174" s="3">
         <v>1121</v>
       </c>
@@ -5467,11 +5470,11 @@
       <c r="F174" s="13" t="s">
         <v>108</v>
       </c>
-      <c r="G174" s="17" t="s">
+      <c r="H174" s="17" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="175" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A175" s="3">
         <v>1129</v>
       </c>
@@ -5490,11 +5493,11 @@
       <c r="F175" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="G175" s="17" t="s">
+      <c r="H175" s="17" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="176" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A176" s="3">
         <v>1132</v>
       </c>
@@ -5513,11 +5516,11 @@
       <c r="F176" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="G176" s="17" t="s">
+      <c r="H176" s="17" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="177" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A177" s="3">
         <v>1135</v>
       </c>
@@ -5536,11 +5539,11 @@
       <c r="F177" s="13" t="s">
         <v>108</v>
       </c>
-      <c r="G177" s="17" t="s">
+      <c r="H177" s="17" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="178" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A178" s="3">
         <v>1142</v>
       </c>
@@ -5559,11 +5562,11 @@
       <c r="F178" s="12" t="s">
         <v>238</v>
       </c>
-      <c r="G178" s="17" t="s">
+      <c r="H178" s="17" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="179" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A179" s="3">
         <v>1144</v>
       </c>
@@ -5582,11 +5585,11 @@
       <c r="F179" s="13" t="s">
         <v>109</v>
       </c>
-      <c r="G179" s="17" t="s">
+      <c r="H179" s="17" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="180" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A180" s="3">
         <v>1167</v>
       </c>
@@ -5605,11 +5608,11 @@
       <c r="F180" s="13" t="s">
         <v>59</v>
       </c>
-      <c r="G180" s="17" t="s">
+      <c r="H180" s="17" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="181" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A181" s="3">
         <v>1191</v>
       </c>
@@ -5628,11 +5631,11 @@
       <c r="F181" s="13" t="s">
         <v>59</v>
       </c>
-      <c r="G181" s="17" t="s">
+      <c r="H181" s="17" t="s">
         <v>239</v>
       </c>
     </row>
-    <row r="182" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A182" s="3">
         <v>1197</v>
       </c>
@@ -5651,11 +5654,11 @@
       <c r="F182" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="G182" s="17" t="s">
+      <c r="H182" s="17" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="183" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A183" s="3">
         <v>1198</v>
       </c>
@@ -5674,11 +5677,11 @@
       <c r="F183" s="13" t="s">
         <v>105</v>
       </c>
-      <c r="G183" s="17" t="s">
+      <c r="H183" s="17" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="184" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A184" s="3">
         <v>1228</v>
       </c>
@@ -5697,11 +5700,11 @@
       <c r="F184" s="13" t="s">
         <v>65</v>
       </c>
-      <c r="G184" s="17" t="s">
+      <c r="H184" s="17" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="185" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A185" s="3">
         <v>1236</v>
       </c>
@@ -5720,11 +5723,11 @@
       <c r="F185" s="13" t="s">
         <v>161</v>
       </c>
-      <c r="G185" s="24" t="s">
+      <c r="H185" s="24" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="186" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A186" s="3">
         <v>1242</v>
       </c>
@@ -5743,11 +5746,11 @@
       <c r="F186" s="13" t="s">
         <v>76</v>
       </c>
-      <c r="G186" s="17" t="s">
+      <c r="H186" s="17" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="187" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A187" s="3">
         <v>1250</v>
       </c>
@@ -5766,11 +5769,11 @@
       <c r="F187" s="19" t="s">
         <v>20</v>
       </c>
-      <c r="G187" s="17" t="s">
+      <c r="H187" s="17" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="188" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A188" s="3">
         <v>1255</v>
       </c>
@@ -5789,11 +5792,11 @@
       <c r="F188" s="13" t="s">
         <v>159</v>
       </c>
-      <c r="G188" s="13" t="s">
+      <c r="H188" s="13" t="s">
         <v>188</v>
       </c>
     </row>
-    <row r="189" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A189" s="3">
         <v>1257</v>
       </c>
@@ -5812,11 +5815,11 @@
       <c r="F189" s="13" t="s">
         <v>40</v>
       </c>
-      <c r="G189" s="17" t="s">
+      <c r="H189" s="17" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="190" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A190" s="3">
         <v>1258</v>
       </c>
@@ -5835,11 +5838,11 @@
       <c r="F190" s="13" t="s">
         <v>40</v>
       </c>
-      <c r="G190" s="17" t="s">
+      <c r="H190" s="17" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="191" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A191" s="3">
         <v>1259</v>
       </c>
@@ -5858,11 +5861,11 @@
       <c r="F191" s="13" t="s">
         <v>40</v>
       </c>
-      <c r="G191" s="17" t="s">
+      <c r="H191" s="17" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="192" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A192" s="3">
         <v>1262</v>
       </c>
@@ -5881,11 +5884,11 @@
       <c r="F192" s="13" t="s">
         <v>254</v>
       </c>
-      <c r="G192" s="17" t="s">
+      <c r="H192" s="17" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="193" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A193" s="3">
         <v>1274</v>
       </c>
@@ -5904,11 +5907,11 @@
       <c r="F193" s="13" t="s">
         <v>187</v>
       </c>
-      <c r="G193" s="17" t="s">
+      <c r="H193" s="17" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="194" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A194" s="3">
         <v>1297</v>
       </c>
@@ -5927,11 +5930,11 @@
       <c r="F194" s="13" t="s">
         <v>105</v>
       </c>
-      <c r="G194" s="17" t="s">
+      <c r="H194" s="17" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="195" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A195" s="3">
         <v>1312</v>
       </c>
@@ -5950,11 +5953,11 @@
       <c r="F195" s="13" t="s">
         <v>105</v>
       </c>
-      <c r="G195" s="17" t="s">
+      <c r="H195" s="17" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="196" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A196" s="3">
         <v>1323</v>
       </c>
@@ -5973,11 +5976,11 @@
       <c r="F196" s="13" t="s">
         <v>105</v>
       </c>
-      <c r="G196" s="17" t="s">
+      <c r="H196" s="17" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="197" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A197" s="3">
         <v>1328</v>
       </c>
@@ -5996,11 +5999,11 @@
       <c r="F197" s="13" t="s">
         <v>108</v>
       </c>
-      <c r="G197" s="17" t="s">
+      <c r="H197" s="17" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="198" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A198" s="3">
         <v>1337</v>
       </c>
@@ -6019,11 +6022,11 @@
       <c r="F198" s="13" t="s">
         <v>107</v>
       </c>
-      <c r="G198" s="17" t="s">
+      <c r="H198" s="17" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="199" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A199" s="3">
         <v>1413</v>
       </c>
@@ -6042,11 +6045,11 @@
       <c r="F199" s="13" t="s">
         <v>59</v>
       </c>
-      <c r="G199" s="17" t="s">
+      <c r="H199" s="17" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="200" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A200" s="3">
         <v>1416</v>
       </c>
@@ -6065,11 +6068,11 @@
       <c r="F200" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="G200" s="17" t="s">
+      <c r="H200" s="17" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="201" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A201" s="3">
         <v>1418</v>
       </c>
@@ -6088,11 +6091,11 @@
       <c r="F201" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="G201" s="19" t="s">
+      <c r="H201" s="19" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="202" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A202" s="3">
         <v>1424</v>
       </c>
@@ -6111,11 +6114,11 @@
       <c r="F202" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="G202" s="17" t="s">
+      <c r="H202" s="17" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="203" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A203" s="3">
         <v>1427</v>
       </c>
@@ -6134,11 +6137,11 @@
       <c r="F203" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="G203" s="17" t="s">
+      <c r="H203" s="17" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="204" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A204" s="3">
         <v>1439</v>
       </c>
@@ -6157,11 +6160,11 @@
       <c r="F204" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="G204" s="17" t="s">
+      <c r="H204" s="17" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="205" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A205" s="3">
         <v>1454</v>
       </c>
@@ -6180,11 +6183,11 @@
       <c r="F205" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="G205" s="17" t="s">
+      <c r="H205" s="17" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="206" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A206" s="3">
         <v>1457</v>
       </c>
@@ -6203,11 +6206,11 @@
       <c r="F206" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="G206" s="17" t="s">
+      <c r="H206" s="17" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="207" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A207" s="3">
         <v>1458</v>
       </c>
@@ -6226,11 +6229,11 @@
       <c r="F207" s="13" t="s">
         <v>159</v>
       </c>
-      <c r="G207" s="17" t="s">
+      <c r="H207" s="17" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="208" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A208" s="3">
         <v>1469</v>
       </c>
@@ -6249,11 +6252,11 @@
       <c r="F208" s="13" t="s">
         <v>221</v>
       </c>
-      <c r="G208" s="17" t="s">
+      <c r="H208" s="17" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="209" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A209" s="3">
         <v>1474</v>
       </c>
@@ -6272,11 +6275,11 @@
       <c r="F209" s="19" t="s">
         <v>20</v>
       </c>
-      <c r="G209" s="19" t="s">
+      <c r="H209" s="19" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="210" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A210" s="3">
         <v>1479</v>
       </c>
@@ -6295,11 +6298,11 @@
       <c r="F210" s="13" t="s">
         <v>109</v>
       </c>
-      <c r="G210" s="17" t="s">
+      <c r="H210" s="17" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="211" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A211" s="3">
         <v>1481</v>
       </c>
@@ -6318,11 +6321,11 @@
       <c r="F211" s="13" t="s">
         <v>222</v>
       </c>
-      <c r="G211" s="17" t="s">
+      <c r="H211" s="17" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="212" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A212" s="3">
         <v>1491</v>
       </c>
@@ -6341,11 +6344,11 @@
       <c r="F212" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="G212" s="17" t="s">
+      <c r="H212" s="17" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="213" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A213" s="3">
         <v>1497</v>
       </c>
@@ -6364,11 +6367,11 @@
       <c r="F213" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="G213" s="17" t="s">
+      <c r="H213" s="17" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="214" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A214" s="3">
         <v>1502</v>
       </c>
@@ -6387,11 +6390,11 @@
       <c r="F214" s="13" t="s">
         <v>222</v>
       </c>
-      <c r="G214" s="17" t="s">
+      <c r="H214" s="17" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="215" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A215" s="3">
         <v>1511</v>
       </c>
@@ -6410,11 +6413,11 @@
       <c r="F215" s="13" t="s">
         <v>40</v>
       </c>
-      <c r="G215" s="17" t="s">
+      <c r="H215" s="17" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="216" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A216" s="3">
         <v>1546</v>
       </c>
@@ -6433,11 +6436,11 @@
       <c r="F216" s="13" t="s">
         <v>160</v>
       </c>
-      <c r="G216" s="13" t="s">
+      <c r="H216" s="13" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="217" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A217" s="3">
         <v>1550</v>
       </c>
@@ -6456,11 +6459,11 @@
       <c r="F217" s="13" t="s">
         <v>105</v>
       </c>
-      <c r="G217" s="13" t="s">
+      <c r="H217" s="13" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="218" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A218" s="3">
         <v>1551</v>
       </c>
@@ -6479,11 +6482,11 @@
       <c r="F218" s="13" t="s">
         <v>105</v>
       </c>
-      <c r="G218" s="17" t="s">
+      <c r="H218" s="17" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="219" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A219" s="3">
         <v>1586</v>
       </c>
@@ -6502,11 +6505,11 @@
       <c r="F219" s="13" t="s">
         <v>160</v>
       </c>
-      <c r="G219" s="13" t="s">
+      <c r="H219" s="13" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="220" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A220" s="3">
         <v>1628</v>
       </c>
@@ -6525,11 +6528,11 @@
       <c r="F220" s="13" t="s">
         <v>217</v>
       </c>
-      <c r="G220" s="17" t="s">
+      <c r="H220" s="17" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="221" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A221" s="3">
         <v>1669</v>
       </c>
@@ -6548,11 +6551,11 @@
       <c r="F221" s="13" t="s">
         <v>105</v>
       </c>
-      <c r="G221" s="17" t="s">
+      <c r="H221" s="17" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="222" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A222" s="3">
         <v>1694</v>
       </c>
@@ -6571,11 +6574,11 @@
       <c r="F222" s="13" t="s">
         <v>103</v>
       </c>
-      <c r="G222" s="17" t="s">
+      <c r="H222" s="17" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="223" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A223" s="3">
         <v>1717</v>
       </c>
@@ -6594,11 +6597,11 @@
       <c r="F223" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="G223" s="17" t="s">
+      <c r="H223" s="17" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="224" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A224" s="3">
         <v>1727</v>
       </c>
@@ -6617,11 +6620,11 @@
       <c r="F224" s="13" t="s">
         <v>105</v>
       </c>
-      <c r="G224" s="17" t="s">
+      <c r="H224" s="17" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="225" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A225" s="3">
         <v>1753</v>
       </c>
@@ -6640,11 +6643,11 @@
       <c r="F225" s="13" t="s">
         <v>59</v>
       </c>
-      <c r="G225" s="17" t="s">
+      <c r="H225" s="17" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="226" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A226" s="3">
         <v>1758</v>
       </c>
@@ -6663,11 +6666,11 @@
       <c r="F226" s="13" t="s">
         <v>222</v>
       </c>
-      <c r="G226" s="17" t="s">
+      <c r="H226" s="17" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="227" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A227" s="3">
         <v>1770</v>
       </c>
@@ -6686,11 +6689,11 @@
       <c r="F227" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="G227" s="17" t="s">
+      <c r="H227" s="17" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="228" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A228" s="3">
         <v>1795</v>
       </c>
@@ -6709,11 +6712,11 @@
       <c r="F228" s="13" t="s">
         <v>160</v>
       </c>
-      <c r="G228" s="17" t="s">
+      <c r="H228" s="17" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="229" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A229" s="3">
         <v>1797</v>
       </c>
@@ -6732,11 +6735,11 @@
       <c r="F229" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="G229" s="27" t="s">
+      <c r="H229" s="27" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="230" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A230" s="3">
         <v>1798</v>
       </c>
@@ -6755,11 +6758,11 @@
       <c r="F230" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="G230" s="27" t="s">
+      <c r="H230" s="27" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="231" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A231" s="3">
         <v>1799</v>
       </c>
@@ -6778,11 +6781,11 @@
       <c r="F231" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="G231" s="27" t="s">
+      <c r="H231" s="27" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="232" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A232" s="3">
         <v>1814</v>
       </c>
@@ -6801,11 +6804,11 @@
       <c r="F232" s="13" t="s">
         <v>222</v>
       </c>
-      <c r="G232" s="17" t="s">
+      <c r="H232" s="17" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="233" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="233" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A233" s="3">
         <v>1827</v>
       </c>
@@ -6824,11 +6827,11 @@
       <c r="F233" s="13" t="s">
         <v>222</v>
       </c>
-      <c r="G233" s="17" t="s">
+      <c r="H233" s="17" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="234" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="234" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A234" s="3">
         <v>1847</v>
       </c>
@@ -6847,11 +6850,11 @@
       <c r="F234" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="G234" s="17" t="s">
+      <c r="H234" s="17" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="235" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="235" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A235" s="3">
         <v>1852</v>
       </c>
@@ -6870,11 +6873,11 @@
       <c r="F235" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="G235" s="17" t="s">
+      <c r="H235" s="17" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="236" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="236" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A236" s="3">
         <v>1856</v>
       </c>
@@ -6893,11 +6896,11 @@
       <c r="F236" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="G236" s="17" t="s">
+      <c r="H236" s="17" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="237" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="237" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A237" s="3">
         <v>1861</v>
       </c>
@@ -6916,11 +6919,11 @@
       <c r="F237" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="G237" s="17" t="s">
+      <c r="H237" s="17" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="238" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="238" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A238" s="3">
         <v>1875</v>
       </c>
@@ -6939,11 +6942,11 @@
       <c r="F238" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="G238" s="17" t="s">
+      <c r="H238" s="17" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="239" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="239" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A239" s="3">
         <v>1888</v>
       </c>
@@ -6962,11 +6965,11 @@
       <c r="F239" s="13" t="s">
         <v>59</v>
       </c>
-      <c r="G239" s="17" t="s">
+      <c r="H239" s="17" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="240" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="240" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A240" s="3">
         <v>1909</v>
       </c>
@@ -6985,11 +6988,11 @@
       <c r="F240" s="13" t="s">
         <v>222</v>
       </c>
-      <c r="G240" s="17" t="s">
+      <c r="H240" s="17" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="241" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="241" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A241" s="3">
         <v>1914</v>
       </c>
@@ -7008,11 +7011,11 @@
       <c r="F241" s="13" t="s">
         <v>222</v>
       </c>
-      <c r="G241" s="17" t="s">
+      <c r="H241" s="17" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="242" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="242" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A242" s="3">
         <v>1919</v>
       </c>
@@ -7031,11 +7034,11 @@
       <c r="F242" s="13" t="s">
         <v>222</v>
       </c>
-      <c r="G242" s="17" t="s">
+      <c r="H242" s="17" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="243" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="243" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A243" s="3">
         <v>1926</v>
       </c>
@@ -7054,11 +7057,11 @@
       <c r="F243" s="13" t="s">
         <v>59</v>
       </c>
-      <c r="G243" s="17" t="s">
+      <c r="H243" s="17" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="244" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="244" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A244" s="3">
         <v>1943</v>
       </c>
@@ -7077,11 +7080,11 @@
       <c r="F244" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="G244" s="17" t="s">
+      <c r="H244" s="17" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="245" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="245" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A245" s="3">
         <v>1953</v>
       </c>
@@ -7100,11 +7103,11 @@
       <c r="F245" s="13" t="s">
         <v>159</v>
       </c>
-      <c r="G245" s="17" t="s">
+      <c r="H245" s="17" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="246" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="246" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A246" s="3">
         <v>1954</v>
       </c>
@@ -7123,11 +7126,11 @@
       <c r="F246" s="13" t="s">
         <v>59</v>
       </c>
-      <c r="G246" s="17" t="s">
+      <c r="H246" s="17" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="247" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="247" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A247" s="3">
         <v>1955</v>
       </c>
@@ -7146,11 +7149,11 @@
       <c r="F247" s="13" t="s">
         <v>105</v>
       </c>
-      <c r="G247" s="17" t="s">
+      <c r="H247" s="17" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="248" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="248" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A248" s="3">
         <v>1962</v>
       </c>
@@ -7169,11 +7172,11 @@
       <c r="F248" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="G248" s="17" t="s">
+      <c r="H248" s="17" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="249" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="249" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A249" s="3">
         <v>1985</v>
       </c>
@@ -7192,11 +7195,11 @@
       <c r="F249" s="13" t="s">
         <v>222</v>
       </c>
-      <c r="G249" s="17" t="s">
+      <c r="H249" s="17" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="250" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="250" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A250" s="3">
         <v>1988</v>
       </c>
@@ -7215,11 +7218,11 @@
       <c r="F250" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="G250" s="17" t="s">
+      <c r="H250" s="17" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="251" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="251" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A251" s="3">
         <v>1990</v>
       </c>
@@ -7238,7 +7241,7 @@
       <c r="F251" s="13" t="s">
         <v>160</v>
       </c>
-      <c r="G251" s="17" t="s">
+      <c r="H251" s="17" t="s">
         <v>129</v>
       </c>
     </row>

</xml_diff>